<commit_message>
clean up per feedback and changes for DM build
</commit_message>
<xml_diff>
--- a/DM Solution Documentation/Recharge Solution Workbook.xlsx
+++ b/DM Solution Documentation/Recharge Solution Workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Documents/DU/Info4240/RechargeVending/DM Solution Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD658A7-BBE1-B944-84FA-6C1DED0E1C91}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF156FE-3CBF-F140-ABCD-A64647EB6B52}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="32620" windowHeight="18200" tabRatio="950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data Warehouse" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Locator">'Data Warehouse'!$LCB$524299</definedName>
+    <definedName name="Locator">'Data Warehouse'!$LCB$524319</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="142">
   <si>
     <t>Object Name</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Dimension Key Column</t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>Dimesion Table</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>nvarchar(30)</t>
   </si>
   <si>
-    <t>nvarchar(20)</t>
-  </si>
-  <si>
     <t>nvarchar(10)</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>DegenerateDimension</t>
   </si>
   <si>
-    <t>RechargeVending.dbo.Stock.Shelf</t>
-  </si>
-  <si>
     <t>RechargeVending.dbo.Stock.Position</t>
   </si>
   <si>
@@ -169,211 +160,295 @@
     <t>nvarchar(75)</t>
   </si>
   <si>
-    <t>RechargeVending.dbo.Product.Size</t>
-  </si>
-  <si>
-    <t>decimal(5,2)</t>
-  </si>
-  <si>
     <t>RechargeVending.dbo.Tender.Name</t>
   </si>
   <si>
-    <t>DWRecharge</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine.Machine_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine.ModelNumber</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine.MachineType</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine.CreditEnabled</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine.MobilePayEnabled</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimMachine.CashEnabled</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation.Location_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation.CampusName</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation.DepartmentName</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation.BuildingName</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation.Floor</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct.Product_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct.ProductType</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct.ProductName</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct.Size</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>DWRecharge.dbo.DimProduct.Brand</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct.Manufacturer</t>
-  </si>
-  <si>
     <t>RechargeVending.dbo.Brand.Name</t>
   </si>
   <si>
     <t>RechargeVending.dbo.Manufacturer.Name</t>
   </si>
   <si>
-    <t>DWRecharge.dbo.DimMachine.Machine_AK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimProduct.Product_AK</t>
-  </si>
-  <si>
     <t>RechargeVending.dbo.ProductType.Description</t>
   </si>
   <si>
     <t>Dimension Table</t>
   </si>
   <si>
-    <t>DWRecharge.dbo.DimDate</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Date</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Year</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Quarter</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.YearQuarter</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Month</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.MonthName</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.WeekOfYear</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.DayofWeek</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.DayName</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Weekend</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Holiday</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Season</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.SaleDate</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Machine_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Location_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Product_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Shelf</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Position</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Tender</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Price</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.Cost</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.FactSale.LastItem</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.Time_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTaime.Second</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.Minute</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.Hour</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.Time</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.AM_PM</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.TimeOfDay</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>nvarchar(2)</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimDate.Date_SK</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimTime.Hour24</t>
-  </si>
-  <si>
-    <t>DWRecharge.dbo.DimLocation.Location_AK</t>
+    <t>RechargeVending.dbo.Stock.Slot</t>
+  </si>
+  <si>
+    <t>RechargeVending.dbo.Sales.SaleTime</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Date_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Date</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.FullDate</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayOfMonth</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayOfWeek</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayOfWeekInMonth</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayOfWeekInYear</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayOfQuarter</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.DayOfYear</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.WeekOfMonth</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.WeekOfQuarter</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.WeekOfYear</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Month</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.MonthName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.MonthOfQuarter</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Quarter</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.QuarterName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Year</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.YearName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.MonthYear</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.MMYYYY</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.FirstDayOfMonth</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.LastDayOfMonth</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.FirstDayOfQuarter</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.LastDayOfQuarter</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.FirstDayOfYear</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.LastDayOfYear</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.IsHoliday</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.IsWeekday</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Holiday</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate.Season</t>
+  </si>
+  <si>
+    <t>nchar(8)</t>
+  </si>
+  <si>
+    <t>nchar(2)</t>
+  </si>
+  <si>
+    <t>nchar(11)</t>
+  </si>
+  <si>
+    <t>nchar(10)</t>
+  </si>
+  <si>
+    <t>nvarchar(9)</t>
+  </si>
+  <si>
+    <t>char(7)</t>
+  </si>
+  <si>
+    <t>char(10)</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>RechargeVending.dbo.SlotSize.Description</t>
+  </si>
+  <si>
+    <t>RechargeDM</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.SaleDate</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.SaleTime</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Machine_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Location_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Product_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Position</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Slot</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Tender</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Price</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Cost</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.LastItem</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.Machine_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.Machine_AK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.ModelName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.MachineType</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.CashEnabled</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.CreditEnabled</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimMachine.MobilePayEnabled</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation.Location_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation.Location_AK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation.CampusName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation.DepartmentName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation.BuildingName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimLocation.Floor</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.Product_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.Product_AK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.ProductType</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.ProductName</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.Brand</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.Manufacturer</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimProduct.Size</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimDate</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.Time_SK</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.Time</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.Hour</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.MilitaryHour</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.Minute</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTaime.Second</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.AmPm</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.DimTime.StandardTime</t>
   </si>
 </sst>
 </file>
@@ -821,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -855,13 +930,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -872,13 +947,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -889,50 +964,50 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
@@ -940,16 +1015,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -957,16 +1032,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>10</v>
@@ -974,13 +1049,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>10</v>
@@ -991,118 +1066,118 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.5" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.5" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>10</v>
@@ -1110,64 +1185,64 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>10</v>
@@ -1178,67 +1253,67 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>10</v>
@@ -1246,118 +1321,118 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="A29" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="5" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>10</v>
@@ -1365,356 +1440,356 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="5" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>77</v>
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="A37" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="6" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="5" t="s">
-        <v>81</v>
+      <c r="A40" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="5" t="s">
-        <v>82</v>
+      <c r="A41" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="5" t="s">
-        <v>83</v>
+      <c r="A42" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="5" t="s">
-        <v>84</v>
+      <c r="A43" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="5" t="s">
-        <v>85</v>
+      <c r="A44" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="5" t="s">
-        <v>86</v>
+      <c r="A45" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="5" t="s">
-        <v>87</v>
+      <c r="A46" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="5" t="s">
-        <v>88</v>
+      <c r="A47" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="5" t="s">
-        <v>89</v>
+      <c r="A48" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="5" t="s">
-        <v>90</v>
+      <c r="A49" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="5" t="s">
-        <v>91</v>
+      <c r="A50" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>7</v>
+      <c r="A51" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="6" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>10</v>
@@ -1722,137 +1797,477 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="6" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="5" t="s">
-        <v>115</v>
+      <c r="A54" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="5" t="s">
-        <v>107</v>
+      <c r="A55" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="5" t="s">
-        <v>106</v>
+      <c r="A56" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="5" t="s">
-        <v>105</v>
+      <c r="A57" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="5" t="s">
-        <v>109</v>
+      <c r="A58" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="5" t="s">
-        <v>110</v>
+      <c r="A59" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ETL & Check Script, Cleaned up Build Script Comments, Added Folder for OLTP Backup FIles.
</commit_message>
<xml_diff>
--- a/DM Solution Documentation/Recharge Solution Workbook.xlsx
+++ b/DM Solution Documentation/Recharge Solution Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Documents/DU/Info4240/RechargeVending/DM Solution Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\RechargeVending\DM Solution Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF156FE-3CBF-F140-ABCD-A64647EB6B52}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{24DEB84A-AD15-47A1-8D19-F12A20390C47}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="32620" windowHeight="18200" tabRatio="950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="383" yWindow="458" windowWidth="32618" windowHeight="18203" tabRatio="950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Warehouse" sheetId="1" r:id="rId1"/>
@@ -334,12 +334,6 @@
     <t>RechargeDM.dbo.FactSale.Product_SK</t>
   </si>
   <si>
-    <t>RechargeDM.dbo.FactSale.Position</t>
-  </si>
-  <si>
-    <t>RechargeDM.dbo.FactSale.Slot</t>
-  </si>
-  <si>
     <t>RechargeDM.dbo.FactSale.Tender</t>
   </si>
   <si>
@@ -449,6 +443,12 @@
   </si>
   <si>
     <t>RechargeDM.dbo.DimTime.StandardTime</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Position_DD</t>
+  </si>
+  <si>
+    <t>RechargeDM.dbo.FactSale.Slot_DD</t>
   </si>
 </sst>
 </file>
@@ -899,16 +899,16 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1049,7 +1049,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>28</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>28</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>28</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>6</v>
@@ -1132,9 +1132,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.5" customHeight="1">
+    <row r="14" spans="1:5" ht="14.55" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>6</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>13</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>13</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>13</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>13</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>13</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>50</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>11</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>13</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>13</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>13</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>13</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>50</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>11</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>13</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>13</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>13</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>13</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>13</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>50</v>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>50</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>13</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>13</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>13</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>13</v>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>13</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>13</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>13</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>13</v>

</xml_diff>